<commit_message>
Tabela IOPC final + Junção JusBrasil e IOPC em um df
</commit_message>
<xml_diff>
--- a/docs/iopc_tables_final.xlsx
+++ b/docs/iopc_tables_final.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,46 +446,38 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Gross Tonnage (GT)</t>
+          <t>Estimated quantity of oil spilled (tonnes)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Estimated quantity of oil spilled (tonnes)</t>
+          <t>Compensation</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Compensation</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
           <t>Currency</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>36506</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>12/12/1999</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>Brittany, France</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>19 666</t>
-        </is>
+      <c r="C2" t="n">
+        <v>19800</v>
       </c>
       <c r="D2" t="n">
-        <v>19800</v>
-      </c>
-      <c r="E2" t="n">
         <v>129712800</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>€</t>
         </is>
@@ -506,18 +494,13 @@
           <t>Piraeus, Greece</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>10 815</t>
-        </is>
+      <c r="C3" t="n">
+        <v>10002500</v>
       </c>
       <c r="D3" t="n">
-        <v>10002500</v>
-      </c>
-      <c r="E3" t="n">
         <v>4022099</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>€</t>
         </is>
@@ -534,18 +517,13 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>42 820</t>
-        </is>
+      <c r="C4" t="n">
+        <v>63200</v>
       </c>
       <c r="D4" t="n">
-        <v>63200</v>
-      </c>
-      <c r="E4" t="n">
         <v>170000000</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>€</t>
         </is>
@@ -559,21 +537,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Namhae, Republic of</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>144</t>
-        </is>
+          <t>Namhae, Republic of Korea</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>100</v>
       </c>
       <c r="D5" t="n">
-        <v>100</v>
-      </c>
-      <c r="E5" t="n">
         <v>3328451732</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>KRW</t>
         </is>
@@ -590,18 +563,13 @@
           <t>Busan, Republic of Korea</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>161</t>
-        </is>
+      <c r="C6" t="n">
+        <v>37</v>
       </c>
       <c r="D6" t="n">
-        <v>37</v>
-      </c>
-      <c r="E6" t="n">
         <v>2044694541</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>KRW</t>
         </is>
@@ -615,21 +583,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Guimaras Strait, Republic of the</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>998</t>
-        </is>
+          <t>Guimaras Strait, Republic of the Philippines</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>2000</v>
       </c>
       <c r="D7" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E7" t="n">
         <v>986646031</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>PHP</t>
         </is>
@@ -646,18 +609,13 @@
           <t>Seto Inland Sea, Japan</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>153</t>
-        </is>
+      <c r="C8" t="n">
+        <v>60</v>
       </c>
       <c r="D8" t="n">
-        <v>60</v>
-      </c>
-      <c r="E8" t="n">
         <v>161064193</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -671,21 +629,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Kerch Strait, between the Sea of Azov and the</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">3 463 </t>
-        </is>
+          <t>Kerch Strait, Russia</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>2000</v>
       </c>
       <c r="D9" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E9" t="n">
         <v>337700000</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>RUB</t>
         </is>
@@ -702,18 +655,13 @@
           <t>Taean, Republic of Korea</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>146 848</t>
-        </is>
+      <c r="C10" t="n">
+        <v>10900</v>
       </c>
       <c r="D10" t="n">
-        <v>10900</v>
-      </c>
-      <c r="E10" t="n">
         <v>182242088000</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>KRW</t>
         </is>
@@ -730,18 +678,13 @@
           <t>Borgå, Finland</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>27 706 GRT</t>
-        </is>
+      <c r="C11" t="n">
+        <v>600700</v>
       </c>
       <c r="D11" t="n">
-        <v>600700</v>
-      </c>
-      <c r="E11" t="n">
-        <v>184992400</v>
-      </c>
-      <c r="F11" t="inlineStr">
+        <v>1849924</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>FM</t>
         </is>
@@ -758,18 +701,13 @@
           <t>Ulsan, Republic of Korea</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>168</t>
-        </is>
+      <c r="C12" t="n">
+        <v>1520</v>
       </c>
       <c r="D12" t="n">
-        <v>1520</v>
-      </c>
-      <c r="E12" t="n">
-        <v>27203317000</v>
-      </c>
-      <c r="F12" t="inlineStr">
+        <v>272033170</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>KRW</t>
         </is>
@@ -783,21 +721,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Hamriyah, Sharjah, United</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>4 233</t>
-        </is>
+          <t>Hamriyah, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>8000</v>
       </c>
       <c r="D13" t="n">
-        <v>8000</v>
-      </c>
-      <c r="E13" t="n">
-        <v>797848300</v>
-      </c>
-      <c r="F13" t="inlineStr">
+        <v>7978483</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>Dhs</t>
         </is>
@@ -814,18 +747,13 @@
           <t>Oki Islands, Japan</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>13 159</t>
-        </is>
+      <c r="C14" t="n">
+        <v>6200</v>
       </c>
       <c r="D14" t="n">
-        <v>6200</v>
-      </c>
-      <c r="E14" t="n">
-        <v>1038916928500</v>
-      </c>
-      <c r="F14" t="inlineStr">
+        <v>10389169285</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -842,18 +770,13 @@
           <t>Otaru, Japan</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>89</t>
-        </is>
+      <c r="C15" t="n">
+        <v>6</v>
       </c>
       <c r="D15" t="n">
-        <v>6</v>
-      </c>
-      <c r="E15" t="n">
-        <v>813132700</v>
-      </c>
-      <c r="F15" t="inlineStr">
+        <v>8131327</v>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -870,18 +793,13 @@
           <t>Kawasaki, Japan</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>186</t>
-        </is>
+      <c r="C16" t="n">
+        <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" t="n">
-        <v>41646540600</v>
-      </c>
-      <c r="F16" t="inlineStr">
+        <v>416465406</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -898,18 +816,13 @@
           <t>Busan, Republic of Korea</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>896</t>
-        </is>
+      <c r="C17" t="n">
+        <v>124</v>
       </c>
       <c r="D17" t="n">
-        <v>124</v>
-      </c>
-      <c r="E17" t="n">
-        <v>47600000000</v>
-      </c>
-      <c r="F17" t="inlineStr">
+        <v>476000000</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>KRW</t>
         </is>
@@ -926,18 +839,13 @@
           <t>Ube, Japan</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>895</t>
-        </is>
+      <c r="C18" t="n">
+        <v>94</v>
       </c>
       <c r="D18" t="n">
-        <v>94</v>
-      </c>
-      <c r="E18" t="n">
-        <v>36657845300</v>
-      </c>
-      <c r="F18" t="inlineStr">
+        <v>366578453</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -954,18 +862,13 @@
           <t>Yosu, Republic of Korea</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>142 488</t>
-        </is>
+      <c r="C19" t="n">
+        <v>1800</v>
       </c>
       <c r="D19" t="n">
-        <v>1800</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1025900000000</v>
-      </c>
-      <c r="F19" t="inlineStr">
+        <v>10259000000</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>KRW</t>
         </is>
@@ -979,21 +882,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Milford Haven, Wales, United</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>77 356</t>
-        </is>
+          <t>Milford Haven, United Kingdom</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>72360</v>
       </c>
       <c r="D20" t="n">
-        <v>72360</v>
-      </c>
-      <c r="E20" t="n">
-        <v>3864151900</v>
-      </c>
-      <c r="F20" t="inlineStr">
+        <v>38641519</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>£</t>
         </is>
@@ -1010,18 +908,13 @@
           <t>Kawasaki, Japan</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>57</t>
-        </is>
+      <c r="C21" t="n">
+        <v>3</v>
       </c>
       <c r="D21" t="n">
-        <v>3</v>
-      </c>
-      <c r="E21" t="n">
-        <v>227846800</v>
-      </c>
-      <c r="F21" t="inlineStr">
+        <v>2278468</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -1035,21 +928,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Agioi Theodoroi,</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>62 678</t>
-        </is>
+          <t>Agioi Theodoroi, Greece</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>30</v>
       </c>
       <c r="D22" t="n">
-        <v>30</v>
-      </c>
-      <c r="E22" t="n">
-        <v>377400000</v>
-      </c>
-      <c r="F22" t="inlineStr">
+        <v>3774000</v>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>€</t>
         </is>
@@ -1066,18 +954,13 @@
           <t>Busan, Republic of Korea</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>560</t>
-        </is>
+      <c r="C23" t="n">
+        <v>28</v>
       </c>
       <c r="D23" t="n">
-        <v>28</v>
-      </c>
-      <c r="E23" t="n">
-        <v>77120858700</v>
-      </c>
-      <c r="F23" t="inlineStr">
+        <v>771208587</v>
+      </c>
+      <c r="E23" t="inlineStr">
         <is>
           <t>KRW</t>
         </is>
@@ -1094,18 +977,13 @@
           <t>Yokohama, Japan</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="C24" t="n">
+        <v>5</v>
       </c>
       <c r="D24" t="n">
-        <v>5</v>
-      </c>
-      <c r="E24" t="n">
-        <v>203394400</v>
-      </c>
-      <c r="F24" t="inlineStr">
+        <v>2033944</v>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -1122,18 +1000,13 @@
           <t>Kainan, Japan</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>2 960</t>
-        </is>
+      <c r="C25" t="n">
+        <v>560</v>
       </c>
       <c r="D25" t="n">
-        <v>560</v>
-      </c>
-      <c r="E25" t="n">
-        <v>71619273700</v>
-      </c>
-      <c r="F25" t="inlineStr">
+        <v>716192737</v>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -1150,18 +1023,13 @@
           <t>Onsan, Republic of Korea</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
+      <c r="C26" t="n">
+        <v>18</v>
       </c>
       <c r="D26" t="n">
-        <v>18</v>
-      </c>
-      <c r="E26" t="n">
-        <v>3778011200</v>
-      </c>
-      <c r="F26" t="inlineStr">
+        <v>37780112</v>
+      </c>
+      <c r="E26" t="inlineStr">
         <is>
           <t>KRW</t>
         </is>
@@ -1175,21 +1043,16 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Kojung, Republic of</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>642</t>
-        </is>
+          <t>Kojung, Republic of Korea</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" t="n">
-        <v>4351712700</v>
-      </c>
-      <c r="F27" t="inlineStr">
+        <v>43517127</v>
+      </c>
+      <c r="E27" t="inlineStr">
         <is>
           <t>KRW</t>
         </is>
@@ -1206,18 +1069,13 @@
           <t>Yosu, Republic of Korea</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>144 567</t>
-        </is>
+      <c r="C28" t="n">
+        <v>5035</v>
       </c>
       <c r="D28" t="n">
-        <v>5035</v>
-      </c>
-      <c r="E28" t="n">
-        <v>5763824413500</v>
-      </c>
-      <c r="F28" t="inlineStr">
+        <v>57638244135</v>
+      </c>
+      <c r="E28" t="inlineStr">
         <is>
           <t>KRW</t>
         </is>
@@ -1234,18 +1092,13 @@
           <t>Yosu, Republic of Korea</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>138</t>
-        </is>
+      <c r="C29" t="n">
+        <v>40</v>
       </c>
       <c r="D29" t="n">
-        <v>40</v>
-      </c>
-      <c r="E29" t="n">
-        <v>155302973900</v>
-      </c>
-      <c r="F29" t="inlineStr">
+        <v>1553029739</v>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t>KRW</t>
         </is>
@@ -1262,18 +1115,13 @@
           <t>Shetland, United Kingdom</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>44 989</t>
-        </is>
+      <c r="C30" t="n">
+        <v>84000</v>
       </c>
       <c r="D30" t="n">
-        <v>84000</v>
-      </c>
-      <c r="E30" t="n">
-        <v>5193893800</v>
-      </c>
-      <c r="F30" t="inlineStr">
+        <v>51938938</v>
+      </c>
+      <c r="E30" t="inlineStr">
         <is>
           <t>£</t>
         </is>
@@ -1290,18 +1138,13 @@
           <t>Tokyo Bay, Japan</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>113</t>
-        </is>
+      <c r="C31" t="n">
+        <v>5</v>
       </c>
       <c r="D31" t="n">
-        <v>5</v>
-      </c>
-      <c r="E31" t="n">
-        <v>182115800</v>
-      </c>
-      <c r="F31" t="inlineStr">
+        <v>1821158</v>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -1318,18 +1161,13 @@
           <t>La Coruña, Spain</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>57 801</t>
-        </is>
+      <c r="C32" t="n">
+        <v>73500</v>
       </c>
       <c r="D32" t="n">
-        <v>73500</v>
-      </c>
-      <c r="E32" t="n">
-        <v>944778678400</v>
-      </c>
-      <c r="F32" t="inlineStr">
+        <v>9447786784</v>
+      </c>
+      <c r="E32" t="inlineStr">
         <is>
           <t>Pts</t>
         </is>
@@ -1346,18 +1184,13 @@
           <t>Tallinn, Estonia</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>949</t>
-        </is>
+      <c r="C33" t="n">
+        <v>140</v>
       </c>
       <c r="D33" t="n">
-        <v>140</v>
-      </c>
-      <c r="E33" t="n">
-        <v>54361800</v>
-      </c>
-      <c r="F33" t="inlineStr">
+        <v>543618</v>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>FM</t>
         </is>
@@ -1374,18 +1207,13 @@
           <t>Seoul, Republic of Korea</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>520</t>
-        </is>
+      <c r="C34" t="n">
+        <v>4</v>
       </c>
       <c r="D34" t="n">
-        <v>4</v>
-      </c>
-      <c r="E34" t="n">
-        <v>21971475500</v>
-      </c>
-      <c r="F34" t="inlineStr">
+        <v>219714755</v>
+      </c>
+      <c r="E34" t="inlineStr">
         <is>
           <t>KRW</t>
         </is>
@@ -1402,18 +1230,13 @@
           <t>Shioyazaki, Japan</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>699</t>
-        </is>
+      <c r="C35" t="n">
+        <v>520</v>
       </c>
       <c r="D35" t="n">
-        <v>520</v>
-      </c>
-      <c r="E35" t="n">
-        <v>110048633500</v>
-      </c>
-      <c r="F35" t="inlineStr">
+        <v>1100486335</v>
+      </c>
+      <c r="E35" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -1430,18 +1253,13 @@
           <t>Izu Peninsula, Japan</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>699</t>
-        </is>
+      <c r="C36" t="n">
+        <v>500</v>
       </c>
       <c r="D36" t="n">
-        <v>500</v>
-      </c>
-      <c r="E36" t="n">
-        <v>1545948100</v>
-      </c>
-      <c r="F36" t="inlineStr">
+        <v>15459481</v>
+      </c>
+      <c r="E36" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -1458,18 +1276,13 @@
           <t>Yeosu, Republic of Korea</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>481</t>
-        </is>
+      <c r="C37" t="n">
+        <v>1280</v>
       </c>
       <c r="D37" t="n">
-        <v>1280</v>
-      </c>
-      <c r="E37" t="n">
-        <v>1628800909900</v>
-      </c>
-      <c r="F37" t="inlineStr">
+        <v>16288009099</v>
+      </c>
+      <c r="E37" t="inlineStr">
         <is>
           <t>KRW</t>
         </is>
@@ -1486,18 +1299,13 @@
           <t>Shiogama, Japan</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>74</t>
-        </is>
+      <c r="C38" t="n">
+        <v>7</v>
       </c>
       <c r="D38" t="n">
-        <v>7</v>
-      </c>
-      <c r="E38" t="n">
-        <v>1990278500</v>
-      </c>
-      <c r="F38" t="inlineStr">
+        <v>19902785</v>
+      </c>
+      <c r="E38" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -1514,18 +1322,13 @@
           <t>Yaizu, Japan</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>174</t>
-        </is>
+      <c r="C39" t="n">
+        <v>2</v>
       </c>
       <c r="D39" t="n">
-        <v>2</v>
-      </c>
-      <c r="E39" t="n">
-        <v>321053000</v>
-      </c>
-      <c r="F39" t="inlineStr">
+        <v>3210530</v>
+      </c>
+      <c r="E39" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -1542,18 +1345,13 @@
           <t>Yokohama, Japan</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>93</t>
-        </is>
+      <c r="C40" t="n">
+        <v>3</v>
       </c>
       <c r="D40" t="n">
-        <v>3</v>
-      </c>
-      <c r="E40" t="n">
-        <v>611441000</v>
-      </c>
-      <c r="F40" t="inlineStr">
+        <v>6114410</v>
+      </c>
+      <c r="E40" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -1570,18 +1368,13 @@
           <t>Osaka, Japan</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>121</t>
-        </is>
+      <c r="C41" t="n">
+        <v>30</v>
       </c>
       <c r="D41" t="n">
-        <v>30</v>
-      </c>
-      <c r="E41" t="n">
         <v>5031266600</v>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -1598,18 +1391,13 @@
           <t>Karlskrona, Sweden</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>3 566</t>
-        </is>
+      <c r="C42" t="n">
+        <v>800</v>
       </c>
       <c r="D42" t="n">
-        <v>800</v>
-      </c>
-      <c r="E42" t="n">
-        <v>1684932800</v>
-      </c>
-      <c r="F42" t="inlineStr">
+        <v>16849328</v>
+      </c>
+      <c r="E42" t="inlineStr">
         <is>
           <t>SEK</t>
         </is>
@@ -1626,18 +1414,13 @@
           <t>Anticosti Island, Canada</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>5 999</t>
-        </is>
+      <c r="C43" t="n">
+        <v>185</v>
       </c>
       <c r="D43" t="n">
-        <v>185</v>
-      </c>
-      <c r="E43" t="n">
-        <v>1283189100</v>
-      </c>
-      <c r="F43" t="inlineStr">
+        <v>12831891</v>
+      </c>
+      <c r="E43" t="inlineStr">
         <is>
           <t>Can$</t>
         </is>
@@ -1651,21 +1434,16 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Pembroke, Wales, United</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>481</t>
-        </is>
+          <t>Pembroke, United Kingdom</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>110</v>
       </c>
       <c r="D44" t="n">
-        <v>110</v>
-      </c>
-      <c r="E44" t="n">
-        <v>27666400</v>
-      </c>
-      <c r="F44" t="inlineStr">
+        <v>276664</v>
+      </c>
+      <c r="E44" t="inlineStr">
         <is>
           <t>£</t>
         </is>
@@ -1682,18 +1460,13 @@
           <t>Nomazaki, Japan</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>499</t>
-        </is>
+      <c r="C45" t="n">
+        <v>25</v>
       </c>
       <c r="D45" t="n">
-        <v>25</v>
-      </c>
-      <c r="E45" t="n">
-        <v>9673293300</v>
-      </c>
-      <c r="F45" t="inlineStr">
+        <v>96732933</v>
+      </c>
+      <c r="E45" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -1710,18 +1483,13 @@
           <t>Ventspils, USSR</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>27 706</t>
-        </is>
+      <c r="C46" t="n">
+        <v>5500</v>
       </c>
       <c r="D46" t="n">
-        <v>5500</v>
-      </c>
-      <c r="E46" t="n">
-        <v>9570716700</v>
-      </c>
-      <c r="F46" t="inlineStr">
+        <v>95707167</v>
+      </c>
+      <c r="E46" t="inlineStr">
         <is>
           <t>Skr</t>
         </is>
@@ -1738,18 +1506,13 @@
           <t>Osaka, Japan</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
+      <c r="C47" t="n">
+        <v>30</v>
       </c>
       <c r="D47" t="n">
-        <v>30</v>
-      </c>
-      <c r="E47" t="n">
-        <v>1685140000</v>
-      </c>
-      <c r="F47" t="inlineStr">
+        <v>16851400</v>
+      </c>
+      <c r="E47" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -1766,18 +1529,13 @@
           <t>Hiroshima, Japan</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>199</t>
-        </is>
+      <c r="C48" t="n">
+        <v>20</v>
       </c>
       <c r="D48" t="n">
-        <v>20</v>
-      </c>
-      <c r="E48" t="n">
-        <v>9545829800</v>
-      </c>
-      <c r="F48" t="inlineStr">
+        <v>95458298</v>
+      </c>
+      <c r="E48" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -1794,18 +1552,13 @@
           <t>Tokyo Bay, Japan</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>68</t>
-        </is>
+      <c r="C49" t="n">
+        <v>80</v>
       </c>
       <c r="D49" t="n">
-        <v>80</v>
-      </c>
-      <c r="E49" t="n">
-        <v>2659866900</v>
-      </c>
-      <c r="F49" t="inlineStr">
+        <v>26598669</v>
+      </c>
+      <c r="E49" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -1822,18 +1575,13 @@
           <t>Aalborg, Denmark</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>1 400</t>
-        </is>
+      <c r="C50" t="n">
+        <v>300</v>
       </c>
       <c r="D50" t="n">
-        <v>300</v>
-      </c>
-      <c r="E50" t="n">
-        <v>984970400</v>
-      </c>
-      <c r="F50" t="inlineStr">
+        <v>9849704</v>
+      </c>
+      <c r="E50" t="inlineStr">
         <is>
           <t>DKr</t>
         </is>
@@ -1850,18 +1598,13 @@
           <t>Elbe Estuary, Germany</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>996</t>
-        </is>
+      <c r="C51" t="n">
+        <v>200</v>
       </c>
       <c r="D51" t="n">
-        <v>200</v>
-      </c>
-      <c r="E51" t="n">
-        <v>322051100</v>
-      </c>
-      <c r="F51" t="inlineStr">
+        <v>3220511</v>
+      </c>
+      <c r="E51" t="inlineStr">
         <is>
           <t>DM</t>
         </is>
@@ -1878,18 +1621,13 @@
           <t>Sakai-Senboku, Japan</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>83</t>
-        </is>
+      <c r="C52" t="n">
+        <v>1</v>
       </c>
       <c r="D52" t="n">
-        <v>1</v>
-      </c>
-      <c r="E52" t="n">
         <v>104987</v>
       </c>
-      <c r="F52" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>€</t>
         </is>
@@ -1906,18 +1644,13 @@
           <t>Gävle, Sweden</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>2 866</t>
-        </is>
+      <c r="C53" t="n">
+        <v>150200</v>
       </c>
       <c r="D53" t="n">
-        <v>150200</v>
-      </c>
-      <c r="E53" t="n">
-        <v>2390306900</v>
-      </c>
-      <c r="F53" t="inlineStr">
+        <v>23903069</v>
+      </c>
+      <c r="E53" t="inlineStr">
         <is>
           <t>SEK</t>
         </is>
@@ -1934,18 +1667,13 @@
           <t>Yawatahama, Japan</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="C54" t="n">
+        <v>25</v>
       </c>
       <c r="D54" t="n">
-        <v>25</v>
-      </c>
-      <c r="E54" t="n">
-        <v>199922500</v>
-      </c>
-      <c r="F54" t="inlineStr">
+        <v>1999225</v>
+      </c>
+      <c r="E54" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -1962,18 +1690,13 @@
           <t>Brittany, France</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>18 325</t>
-        </is>
+      <c r="C55" t="n">
+        <v>2000</v>
       </c>
       <c r="D55" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E55" t="n">
-        <v>128697700</v>
-      </c>
-      <c r="F55" t="inlineStr">
+        <v>1286977</v>
+      </c>
+      <c r="E55" t="inlineStr">
         <is>
           <t>FFr</t>
         </is>
@@ -1990,18 +1713,13 @@
           <t>Yokohama, Japan</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>86</t>
-        </is>
+      <c r="C56" t="n">
+        <v>6</v>
       </c>
       <c r="D56" t="n">
-        <v>6</v>
-      </c>
-      <c r="E56" t="n">
-        <v>675408500</v>
-      </c>
-      <c r="F56" t="inlineStr">
+        <v>6754085</v>
+      </c>
+      <c r="E56" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -2018,18 +1736,13 @@
           <t>Kyoga Misaki, Japan</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>480</t>
-        </is>
+      <c r="C57" t="n">
+        <v>1100</v>
       </c>
       <c r="D57" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E57" t="n">
-        <v>42961892700</v>
-      </c>
-      <c r="F57" t="inlineStr">
+        <v>429618927</v>
+      </c>
+      <c r="E57" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -2046,18 +1759,13 @@
           <t>Bisan Seto, Japan</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>997</t>
-        </is>
+      <c r="C58" t="n">
+        <v>540</v>
       </c>
       <c r="D58" t="n">
-        <v>540</v>
-      </c>
-      <c r="E58" t="n">
-        <v>14953816700</v>
-      </c>
-      <c r="F58" t="inlineStr">
+        <v>149538167</v>
+      </c>
+      <c r="E58" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -2074,18 +1782,13 @@
           <t>Mebaru, Japan</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="C59" t="n">
+        <v>10</v>
       </c>
       <c r="D59" t="n">
-        <v>10</v>
-      </c>
-      <c r="E59" t="n">
-        <v>1039970500</v>
-      </c>
-      <c r="F59" t="inlineStr">
+        <v>10399705</v>
+      </c>
+      <c r="E59" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -2102,18 +1805,13 @@
           <t>Naruto Strait, Japan</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>199</t>
-        </is>
+      <c r="C60" t="n">
+        <v>100</v>
       </c>
       <c r="D60" t="n">
-        <v>100</v>
-      </c>
-      <c r="E60" t="n">
-        <v>10513565900</v>
-      </c>
-      <c r="F60" t="inlineStr">
+        <v>105135659</v>
+      </c>
+      <c r="E60" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -2130,18 +1828,13 @@
           <t>Brittany, France</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>18 048</t>
-        </is>
+      <c r="C61" t="n">
+        <v>13500</v>
       </c>
       <c r="D61" t="n">
-        <v>13500</v>
-      </c>
-      <c r="E61" t="n">
-        <v>22214064300</v>
-      </c>
-      <c r="F61" t="inlineStr">
+        <v>222140643</v>
+      </c>
+      <c r="E61" t="inlineStr">
         <is>
           <t>FFr</t>
         </is>
@@ -2158,18 +1851,13 @@
           <t>Miyagi, Japan</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>983</t>
-        </is>
+      <c r="C62" t="n">
+        <v>270</v>
       </c>
       <c r="D62" t="n">
-        <v>270</v>
-      </c>
-      <c r="E62" t="n">
-        <v>22226434500</v>
-      </c>
-      <c r="F62" t="inlineStr">
+        <v>222264345</v>
+      </c>
+      <c r="E62" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -2186,18 +1874,13 @@
           <t>Karatsu, Japan</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>199</t>
-        </is>
+      <c r="C63" t="n">
+        <v>10</v>
       </c>
       <c r="D63" t="n">
-        <v>10</v>
-      </c>
-      <c r="E63" t="n">
-        <v>827594200</v>
-      </c>
-      <c r="F63" t="inlineStr">
+        <v>8275942</v>
+      </c>
+      <c r="E63" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -2214,20 +1897,15 @@
           <t>Klaipeda, USSR</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>12 404</t>
-        </is>
+      <c r="C64" t="n">
+        <v>16000</v>
       </c>
       <c r="D64" t="n">
-        <v>16000</v>
-      </c>
-      <c r="E64" t="n">
         <v>467953</v>
       </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>US$</t>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>€</t>
         </is>
       </c>
     </row>
@@ -2242,18 +1920,13 @@
           <t>Hamburg, Germany</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>31 030</t>
-        </is>
+      <c r="C65" t="n">
+        <v>200300</v>
       </c>
       <c r="D65" t="n">
-        <v>200300</v>
-      </c>
-      <c r="E65" t="n">
-        <v>1134517400</v>
-      </c>
-      <c r="F65" t="inlineStr">
+        <v>11345174</v>
+      </c>
+      <c r="E65" t="inlineStr">
         <is>
           <t>DM</t>
         </is>
@@ -2270,18 +1943,13 @@
           <t>Takashima Island, Japan</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>161</t>
-        </is>
+      <c r="C66" t="n">
+        <v>20</v>
       </c>
       <c r="D66" t="n">
-        <v>20</v>
-      </c>
-      <c r="E66" t="n">
-        <v>7267178900</v>
-      </c>
-      <c r="F66" t="inlineStr">
+        <v>72671789</v>
+      </c>
+      <c r="E66" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -2298,18 +1966,13 @@
           <t>Tachibana Bay, Japan</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>499</t>
-        </is>
+      <c r="C67" t="n">
+        <v>85</v>
       </c>
       <c r="D67" t="n">
-        <v>85</v>
-      </c>
-      <c r="E67" t="n">
-        <v>36894286500</v>
-      </c>
-      <c r="F67" t="inlineStr">
+        <v>368942865</v>
+      </c>
+      <c r="E67" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -2326,18 +1989,13 @@
           <t>Ishinomaki, Japan</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>107</t>
-        </is>
+      <c r="C68" t="n">
+        <v>33</v>
       </c>
       <c r="D68" t="n">
-        <v>33</v>
-      </c>
-      <c r="E68" t="n">
-        <v>59818100</v>
-      </c>
-      <c r="F68" t="inlineStr">
+        <v>598181</v>
+      </c>
+      <c r="E68" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -2354,18 +2012,13 @@
           <t>Ichikawa, Japan</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
+      <c r="C69" t="n">
+        <v>35</v>
       </c>
       <c r="D69" t="n">
-        <v>35</v>
-      </c>
-      <c r="E69" t="n">
-        <v>147539500</v>
-      </c>
-      <c r="F69" t="inlineStr">
+        <v>1475395</v>
+      </c>
+      <c r="E69" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -2382,18 +2035,13 @@
           <t>Karakuwazaki, Japan</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>999</t>
-        </is>
+      <c r="C70" t="n">
+        <v>357</v>
       </c>
       <c r="D70" t="n">
-        <v>357</v>
-      </c>
-      <c r="E70" t="n">
-        <v>3459658900</v>
-      </c>
-      <c r="F70" t="inlineStr">
+        <v>34596589</v>
+      </c>
+      <c r="E70" t="inlineStr">
         <is>
           <t>¥</t>
         </is>
@@ -2410,18 +2058,13 @@
           <t>Nagoya, Japan</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>82</t>
-        </is>
+      <c r="C71" t="n">
+        <v>49</v>
       </c>
       <c r="D71" t="n">
-        <v>49</v>
-      </c>
-      <c r="E71" t="n">
-        <v>2775516300</v>
-      </c>
-      <c r="F71" t="inlineStr">
+        <v>27755163</v>
+      </c>
+      <c r="E71" t="inlineStr">
         <is>
           <t>¥</t>
         </is>

</xml_diff>